<commit_message>
Do not apply both NCAP_AFA and NCAP_AFC to heating tech in RSD
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0308F661-8C72-417A-8165-567B850378B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD723570-C9BF-4C8D-9D2B-F2DA3D3D252B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="819" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2373,7 +2373,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="IEA Data"/>
@@ -2508,9 +2508,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2548,9 +2548,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2583,26 +2583,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2635,26 +2618,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -11736,7 +11702,9 @@
   </sheetPr>
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11965,8 +11933,8 @@
         <v>244</v>
       </c>
       <c r="B10" s="30" t="str">
-        <f>"R-*_"&amp;F10&amp;"*"&amp;"HPN*"</f>
-        <v>R-*_Apt*HPN*</v>
+        <f>"R-SH_"&amp;F10&amp;"*"&amp;"HPN*"</f>
+        <v>R-SH_Apt*HPN*</v>
       </c>
       <c r="C10" s="30"/>
       <c r="D10" s="53">
@@ -12000,8 +11968,8 @@
         <v>244</v>
       </c>
       <c r="B11" s="31" t="str">
-        <f>"R-S*_"&amp;F11&amp;"_"&amp;G11&amp;"_N1"&amp;",-R-SC*"</f>
-        <v>R-S*_Apt_ELC_N1,-R-SC*</v>
+        <f>"R-SH_"&amp;F11&amp;"_"&amp;G11&amp;"_N1"</f>
+        <v>R-SH_Apt_ELC_N1</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="54">
@@ -12367,8 +12335,8 @@
         <v>244</v>
       </c>
       <c r="B23" s="30" t="str">
-        <f>"R-*_"&amp;F23&amp;"*"&amp;"HPN*"</f>
-        <v>R-*_Att*HPN*</v>
+        <f>"R-SH_"&amp;F23&amp;"*"&amp;"HPN*"</f>
+        <v>R-SH_Att*HPN*</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="53">
@@ -12401,8 +12369,8 @@
         <v>244</v>
       </c>
       <c r="B24" s="31" t="str">
-        <f>"R-S*_"&amp;F24&amp;"_"&amp;G24&amp;"_N1"&amp;",-R-SC*"</f>
-        <v>R-S*_Att_ELC_N1,-R-SC*</v>
+        <f>"R-SH_"&amp;F24&amp;"_"&amp;G24&amp;"_N1"</f>
+        <v>R-SH_Att_ELC_N1</v>
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="54">
@@ -12732,8 +12700,8 @@
         <v>244</v>
       </c>
       <c r="B38" s="30" t="str">
-        <f>"R-*_"&amp;F38&amp;"*"&amp;"HPN*"</f>
-        <v>R-*_Det*HPN*</v>
+        <f>"R-SH_"&amp;F38&amp;"*"&amp;"HPN*"</f>
+        <v>R-SH_Det*HPN*</v>
       </c>
       <c r="C38" s="30"/>
       <c r="D38" s="53">
@@ -12756,8 +12724,8 @@
         <v>244</v>
       </c>
       <c r="B39" s="31" t="str">
-        <f>"R-S*_"&amp;F39&amp;"_"&amp;G39&amp;"_N1"&amp;",-R-SC*"</f>
-        <v>R-S*_Det_ELC_N1,-R-SC*</v>
+        <f>"R-SH_"&amp;F39&amp;"_"&amp;G39&amp;"_N1"</f>
+        <v>R-SH_Det_ELC_N1</v>
       </c>
       <c r="C39" s="31"/>
       <c r="D39" s="54">
@@ -13071,8 +13039,8 @@
         <v>198</v>
       </c>
       <c r="B53" s="30" t="str">
-        <f>"R-*_"&amp;F53&amp;"*"&amp;"HPN*"</f>
-        <v>R-*_Apt*HPN*</v>
+        <f>"R-SW_"&amp;F53&amp;"*"&amp;"HPN*"</f>
+        <v>R-SW_Apt*HPN*</v>
       </c>
       <c r="C53" s="30" t="s">
         <v>296</v>
@@ -13094,11 +13062,11 @@
     </row>
     <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
-        <v>198</v>
+        <v>1</v>
       </c>
       <c r="B54" s="31" t="str">
-        <f>"R-S*_"&amp;F54&amp;"_"&amp;G54&amp;"_N1"&amp;",-R-SC*"</f>
-        <v>R-S*_Apt_ELC_N1,-R-SC*</v>
+        <f>"R-SW_"&amp;F54&amp;"_"&amp;G54&amp;"_N1"</f>
+        <v>R-SW_Apt_ELC_N1</v>
       </c>
       <c r="C54" s="31" t="s">
         <v>296</v>
@@ -13395,8 +13363,8 @@
         <v>198</v>
       </c>
       <c r="B66" s="30" t="str">
-        <f>"R-*_"&amp;F66&amp;"*"&amp;"HPN*"</f>
-        <v>R-*_Att*HPN*</v>
+        <f>"R-SW_"&amp;F66&amp;"*"&amp;"HPN*"</f>
+        <v>R-SW_Att*HPN*</v>
       </c>
       <c r="C66" s="30" t="s">
         <v>298</v>
@@ -13418,11 +13386,11 @@
     </row>
     <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="31" t="s">
-        <v>198</v>
+        <v>1</v>
       </c>
       <c r="B67" s="31" t="str">
-        <f>"R-S*_"&amp;F67&amp;"_"&amp;G67&amp;"_N1"&amp;",-R-SC*"</f>
-        <v>R-S*_Att_ELC_N1,-R-SC*</v>
+        <f>"R-SW_"&amp;F67&amp;"_"&amp;G67&amp;"_N1"</f>
+        <v>R-SW_Att_ELC_N1</v>
       </c>
       <c r="C67" s="31" t="s">
         <v>298</v>
@@ -13755,8 +13723,8 @@
         <v>198</v>
       </c>
       <c r="B81" s="30" t="str">
-        <f>"R-*_"&amp;F81&amp;"*"&amp;"HPN*"</f>
-        <v>R-*_Det*HPN*</v>
+        <f>"R-SW_"&amp;F81&amp;"*"&amp;"HPN*"</f>
+        <v>R-SW_Det*HPN*</v>
       </c>
       <c r="C81" s="30" t="s">
         <v>300</v>
@@ -13778,11 +13746,11 @@
     </row>
     <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="31" t="s">
-        <v>198</v>
+        <v>1</v>
       </c>
       <c r="B82" s="31" t="str">
-        <f>"R-S*_"&amp;F82&amp;"_"&amp;G82&amp;"_N1"&amp;",-R-SC*"</f>
-        <v>R-S*_Det_ELC_N1,-R-SC*</v>
+        <f>"R-SW_"&amp;F82&amp;"_"&amp;G82&amp;"_N1"</f>
+        <v>R-SW_Det_ELC_N1</v>
       </c>
       <c r="C82" s="31" t="s">
         <v>300</v>

</xml_diff>

<commit_message>
Use defined RSD commodity groups to specify NCAP_AFC
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIM\fix-rsd-heating\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF4DF80-97CD-45A5-9889-0448D6F56CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71A90B3-E2B5-4F96-8B68-AE7AAB368FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="3135" windowWidth="21600" windowHeight="11295" tabRatio="819" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="819" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="65" r:id="rId1"/>
@@ -559,7 +559,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2775" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2765" uniqueCount="302">
   <si>
     <t>IE</t>
   </si>
@@ -1335,9 +1335,6 @@
     <t>*Apartment Space Heat (dual techs)</t>
   </si>
   <si>
-    <t>*Space Heating (dual techs)</t>
-  </si>
-  <si>
     <t>R-RSDCK_ELC_X0</t>
   </si>
   <si>
@@ -1464,28 +1461,28 @@
     <t>New Technologies - Transformation</t>
   </si>
   <si>
-    <t>RSDSH_Apt-AB,RSDSH_Apt-C,RSDSH_Apt-D,RSDSH_Apt-E,RSDSH_Apt-F,RSDSH_Apt-G</t>
-  </si>
-  <si>
-    <t>RSDSH_Apt-AB,RSDSH_Apt-C,RSDSH_Apt-D,RSDSH_Apt-E,RSDSH_Apt-F,RSDSH_Apt-G,RSDWH_Apt</t>
-  </si>
-  <si>
-    <t>RSDSH_Att-AB,RSDSH_Att-C,RSDSH_Att-D,RSDSH_Att-E,RSDSH_Att-F,RSDSH_Att-G</t>
-  </si>
-  <si>
-    <t>RSDSH_Att-AB,RSDSH_Att-C,RSDSH_Att-D,RSDSH_Att-E,RSDSH_Att-F,RSDSH_Att-G,RSDWH_Att</t>
-  </si>
-  <si>
-    <t>RSDSH_Det-AB,RSDSH_Det-C,RSDSH_Det-D,RSDSH_Det-E,RSDSH_Det-F,RSDSH_Det-G</t>
-  </si>
-  <si>
-    <t>RSDSH_Det-AB,RSDSH_Det-C,RSDSH_Det-D,RSDSH_Det-E,RSDSH_Det-F,RSDSH_Det-G,RSDWH_Det</t>
-  </si>
-  <si>
     <t>*1</t>
   </si>
   <si>
-    <t>Top_check</t>
+    <t>Other_Indexes</t>
+  </si>
+  <si>
+    <t>RSDSH_Apt,RSDWH_Apt</t>
+  </si>
+  <si>
+    <t>RSDSH_Att,RSDWH_Att</t>
+  </si>
+  <si>
+    <t>RSDSH_Det,RSDWH_Det</t>
+  </si>
+  <si>
+    <t>RSDSH_Apt,RSDSC_Apt</t>
+  </si>
+  <si>
+    <t>RSDSH_Att,RSDSC_Att</t>
+  </si>
+  <si>
+    <t>RSDSH_Det,RSDSC_Det</t>
   </si>
 </sst>
 </file>
@@ -3238,7 +3235,7 @@
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B16" s="58"/>
       <c r="C16" s="58"/>
@@ -3324,10 +3321,10 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C19" s="57"/>
       <c r="D19" s="57"/>
@@ -3356,10 +3353,10 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B20" s="57" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C20" s="57"/>
       <c r="D20" s="57"/>
@@ -3388,10 +3385,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B21" s="48" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C21" s="48"/>
       <c r="D21" s="48"/>
@@ -3448,10 +3445,10 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C23" s="57"/>
       <c r="D23" s="57"/>
@@ -3481,7 +3478,7 @@
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="45"/>
       <c r="B24" s="57" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C24" s="57"/>
       <c r="D24" s="57"/>
@@ -3511,7 +3508,7 @@
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="45"/>
       <c r="B25" s="57" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C25" s="57"/>
       <c r="D25" s="57"/>
@@ -3540,10 +3537,10 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="45" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B26" s="57" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C26" s="57"/>
       <c r="D26" s="57"/>
@@ -3573,7 +3570,7 @@
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="45"/>
       <c r="B27" s="57" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C27" s="57"/>
       <c r="D27" s="57"/>
@@ -3630,7 +3627,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="45" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B29" s="49">
         <v>1</v>
@@ -3662,10 +3659,10 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="45" t="s">
+        <v>283</v>
+      </c>
+      <c r="B30" s="59" t="s">
         <v>284</v>
-      </c>
-      <c r="B30" s="59" t="s">
-        <v>285</v>
       </c>
       <c r="C30" s="57"/>
       <c r="D30" s="57"/>
@@ -3694,10 +3691,10 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="B31" s="57" t="s">
         <v>286</v>
-      </c>
-      <c r="B31" s="57" t="s">
-        <v>287</v>
       </c>
       <c r="C31" s="57"/>
       <c r="D31" s="57"/>
@@ -3727,7 +3724,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="51"/>
       <c r="B32" s="52" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C32" s="51"/>
       <c r="D32" s="51"/>
@@ -6411,7 +6408,7 @@
         <v>177</v>
       </c>
       <c r="C19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D19" t="s">
         <v>131</v>
@@ -6452,7 +6449,7 @@
         <v>177</v>
       </c>
       <c r="C20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D20" t="s">
         <v>131</v>
@@ -6493,7 +6490,7 @@
         <v>177</v>
       </c>
       <c r="C21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D21" t="s">
         <v>131</v>
@@ -6575,7 +6572,7 @@
         <v>177</v>
       </c>
       <c r="C23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D23" t="s">
         <v>131</v>
@@ -6616,7 +6613,7 @@
         <v>177</v>
       </c>
       <c r="C24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D24" t="s">
         <v>131</v>
@@ -6657,7 +6654,7 @@
         <v>177</v>
       </c>
       <c r="C25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D25" t="s">
         <v>131</v>
@@ -6903,7 +6900,7 @@
         <v>177</v>
       </c>
       <c r="C31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D31" t="s">
         <v>131</v>
@@ -6944,7 +6941,7 @@
         <v>177</v>
       </c>
       <c r="C32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D32" t="s">
         <v>131</v>
@@ -6985,7 +6982,7 @@
         <v>177</v>
       </c>
       <c r="C33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D33" t="s">
         <v>131</v>
@@ -7067,7 +7064,7 @@
         <v>177</v>
       </c>
       <c r="C35" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D35" t="s">
         <v>131</v>
@@ -7108,7 +7105,7 @@
         <v>177</v>
       </c>
       <c r="C36" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D36" t="s">
         <v>131</v>
@@ -7149,7 +7146,7 @@
         <v>177</v>
       </c>
       <c r="C37" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D37" t="s">
         <v>131</v>
@@ -8707,7 +8704,7 @@
         <v>177</v>
       </c>
       <c r="C75" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D75" t="s">
         <v>131</v>
@@ -9493,7 +9490,7 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D2" t="s">
         <v>131</v>
@@ -9534,7 +9531,7 @@
         <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D3" t="s">
         <v>131</v>
@@ -9575,7 +9572,7 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D4" t="s">
         <v>131</v>
@@ -11703,18 +11700,18 @@
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:M141"/>
+  <dimension ref="A1:M137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="21" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="21" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" style="21" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" style="21" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" style="21" customWidth="1"/>
@@ -11755,7 +11752,7 @@
         <v>76</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="E4" s="23" t="s">
         <v>72</v>
@@ -12465,7 +12462,7 @@
         <v>244</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
@@ -12585,7 +12582,7 @@
         <v>244</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C31" s="30"/>
       <c r="D31" s="30"/>
@@ -12815,7 +12812,7 @@
         <v>244</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C41" s="31"/>
       <c r="D41" s="31"/>
@@ -12932,7 +12929,7 @@
         <v>244</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C46" s="30"/>
       <c r="D46" s="30"/>
@@ -12989,11 +12986,9 @@
         <f>"R-SW*"&amp;G49&amp;"_"&amp;H49&amp;"*"</f>
         <v>R-SW*Apt_COA*</v>
       </c>
-      <c r="C49" s="30" t="s">
+      <c r="C49" s="30"/>
+      <c r="D49" s="30" t="s">
         <v>296</v>
-      </c>
-      <c r="D49" s="30">
-        <v>1</v>
       </c>
       <c r="E49" s="53">
         <f>E6</f>
@@ -13018,11 +13013,9 @@
         <f>"R-SW*"&amp;G50&amp;"_"&amp;H50&amp;"*"</f>
         <v>R-SW*Apt_BDL*</v>
       </c>
-      <c r="C50" s="31" t="s">
+      <c r="C50" s="31"/>
+      <c r="D50" s="31" t="s">
         <v>296</v>
-      </c>
-      <c r="D50" s="31">
-        <v>1</v>
       </c>
       <c r="E50" s="54">
         <f t="shared" ref="E50:E59" si="9">E7</f>
@@ -13047,11 +13040,9 @@
         <f>"R-SW*"&amp;G51&amp;"_"&amp;H51&amp;"*"</f>
         <v>R-SW*Apt_ETH*</v>
       </c>
-      <c r="C51" s="30" t="s">
+      <c r="C51" s="30"/>
+      <c r="D51" s="30" t="s">
         <v>296</v>
-      </c>
-      <c r="D51" s="30">
-        <v>1</v>
       </c>
       <c r="E51" s="53">
         <f t="shared" si="9"/>
@@ -13076,11 +13067,9 @@
         <f>"R-SW*"&amp;G52&amp;"_"&amp;H52&amp;"*"</f>
         <v>R-SW*Apt_LPG*</v>
       </c>
-      <c r="C52" s="31" t="s">
+      <c r="C52" s="31"/>
+      <c r="D52" s="31" t="s">
         <v>296</v>
-      </c>
-      <c r="D52" s="31">
-        <v>1</v>
       </c>
       <c r="E52" s="54">
         <f t="shared" si="9"/>
@@ -13105,11 +13094,9 @@
         <f>"R-SW_"&amp;G53&amp;"*"&amp;"HPN*"</f>
         <v>R-SW_Apt*HPN*</v>
       </c>
-      <c r="C53" s="30" t="s">
+      <c r="C53" s="30"/>
+      <c r="D53" s="30" t="s">
         <v>296</v>
-      </c>
-      <c r="D53" s="30">
-        <v>1</v>
       </c>
       <c r="E53" s="53">
         <f>E10</f>
@@ -13134,11 +13121,9 @@
         <f>"R-SW_"&amp;G54&amp;"_"&amp;H54&amp;"_N1"</f>
         <v>R-SW_Apt_ELC_N1</v>
       </c>
-      <c r="C54" s="31" t="s">
+      <c r="C54" s="31"/>
+      <c r="D54" s="31" t="s">
         <v>296</v>
-      </c>
-      <c r="D54" s="31">
-        <v>1</v>
       </c>
       <c r="E54" s="54">
         <f t="shared" si="9"/>
@@ -13163,11 +13148,9 @@
         <f t="shared" ref="B55:B60" si="10">"R-SW*"&amp;G55&amp;"_"&amp;H55&amp;"*"</f>
         <v>R-SW*Apt_KER*</v>
       </c>
-      <c r="C55" s="30" t="s">
+      <c r="C55" s="30"/>
+      <c r="D55" s="30" t="s">
         <v>296</v>
-      </c>
-      <c r="D55" s="30">
-        <v>1</v>
       </c>
       <c r="E55" s="53">
         <f t="shared" si="9"/>
@@ -13192,11 +13175,9 @@
         <f t="shared" si="10"/>
         <v>R-SW*Apt_GAS*</v>
       </c>
-      <c r="C56" s="31" t="s">
+      <c r="C56" s="31"/>
+      <c r="D56" s="31" t="s">
         <v>296</v>
-      </c>
-      <c r="D56" s="31">
-        <v>1</v>
       </c>
       <c r="E56" s="54">
         <f t="shared" si="9"/>
@@ -13221,11 +13202,9 @@
         <f t="shared" si="10"/>
         <v>R-SW*Apt_PEA*</v>
       </c>
-      <c r="C57" s="30" t="s">
+      <c r="C57" s="30"/>
+      <c r="D57" s="30" t="s">
         <v>296</v>
-      </c>
-      <c r="D57" s="30">
-        <v>1</v>
       </c>
       <c r="E57" s="53">
         <f t="shared" si="9"/>
@@ -13250,11 +13229,9 @@
         <f t="shared" si="10"/>
         <v>R-SW*Apt_SMF*</v>
       </c>
-      <c r="C58" s="31" t="s">
+      <c r="C58" s="31"/>
+      <c r="D58" s="31" t="s">
         <v>296</v>
-      </c>
-      <c r="D58" s="31">
-        <v>1</v>
       </c>
       <c r="E58" s="54">
         <f t="shared" si="9"/>
@@ -13279,11 +13256,9 @@
         <f t="shared" si="10"/>
         <v>R-SW*Apt_WOO*</v>
       </c>
-      <c r="C59" s="30" t="s">
+      <c r="C59" s="30"/>
+      <c r="D59" s="30" t="s">
         <v>296</v>
-      </c>
-      <c r="D59" s="30">
-        <v>1</v>
       </c>
       <c r="E59" s="53">
         <f t="shared" si="9"/>
@@ -13308,11 +13283,9 @@
         <f t="shared" si="10"/>
         <v>R-SW*Apt_HET*</v>
       </c>
-      <c r="C60" s="31" t="s">
+      <c r="C60" s="31"/>
+      <c r="D60" s="31" t="s">
         <v>296</v>
-      </c>
-      <c r="D60" s="31">
-        <v>1</v>
       </c>
       <c r="E60" s="54">
         <f>E17</f>
@@ -13350,11 +13323,9 @@
         <f>"R-SW*"&amp;G62&amp;"_"&amp;H62&amp;"*"</f>
         <v>R-SW*Att_COA*</v>
       </c>
-      <c r="C62" s="30" t="s">
-        <v>298</v>
-      </c>
-      <c r="D62" s="30">
-        <v>1</v>
+      <c r="C62" s="30"/>
+      <c r="D62" s="30" t="s">
+        <v>297</v>
       </c>
       <c r="E62" s="53">
         <f>E19</f>
@@ -13379,11 +13350,9 @@
         <f>"R-SW*"&amp;G63&amp;"_"&amp;H63&amp;"*"</f>
         <v>R-SW*Att_BDL*</v>
       </c>
-      <c r="C63" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="D63" s="31">
-        <v>1</v>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31" t="s">
+        <v>297</v>
       </c>
       <c r="E63" s="54">
         <f t="shared" ref="E63:E75" si="13">E20</f>
@@ -13408,11 +13377,9 @@
         <f>"R-SW*"&amp;G64&amp;"_"&amp;H64&amp;"*"</f>
         <v>R-SW*Att_ETH*</v>
       </c>
-      <c r="C64" s="30" t="s">
-        <v>298</v>
-      </c>
-      <c r="D64" s="30">
-        <v>1</v>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30" t="s">
+        <v>297</v>
       </c>
       <c r="E64" s="53">
         <f t="shared" si="13"/>
@@ -13437,11 +13404,9 @@
         <f>"R-SW*"&amp;G65&amp;"_"&amp;H65&amp;"*"</f>
         <v>R-SW*Att_LPG*</v>
       </c>
-      <c r="C65" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="D65" s="31">
-        <v>1</v>
+      <c r="C65" s="31"/>
+      <c r="D65" s="31" t="s">
+        <v>297</v>
       </c>
       <c r="E65" s="54">
         <f t="shared" si="13"/>
@@ -13466,11 +13431,9 @@
         <f>"R-SW_"&amp;G66&amp;"*"&amp;"HPN*"</f>
         <v>R-SW_Att*HPN*</v>
       </c>
-      <c r="C66" s="30" t="s">
-        <v>298</v>
-      </c>
-      <c r="D66" s="30">
-        <v>1</v>
+      <c r="C66" s="30"/>
+      <c r="D66" s="30" t="s">
+        <v>297</v>
       </c>
       <c r="E66" s="53">
         <f t="shared" si="13"/>
@@ -13495,11 +13458,9 @@
         <f>"R-SW_"&amp;G67&amp;"_"&amp;H67&amp;"_N1"</f>
         <v>R-SW_Att_ELC_N1</v>
       </c>
-      <c r="C67" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="D67" s="31">
-        <v>1</v>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31" t="s">
+        <v>297</v>
       </c>
       <c r="E67" s="54">
         <f t="shared" si="13"/>
@@ -13524,11 +13485,9 @@
         <f t="shared" ref="B68:B75" si="14">"R-SW*"&amp;G68&amp;"_"&amp;H68&amp;"*"</f>
         <v>R-SW*Att_KER*</v>
       </c>
-      <c r="C68" s="30" t="s">
-        <v>298</v>
-      </c>
-      <c r="D68" s="30">
-        <v>1</v>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30" t="s">
+        <v>297</v>
       </c>
       <c r="E68" s="53">
         <f t="shared" si="13"/>
@@ -13550,13 +13509,11 @@
         <v>198</v>
       </c>
       <c r="B69" s="31" t="s">
-        <v>275</v>
-      </c>
-      <c r="C69" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="D69" s="31">
-        <v>1</v>
+        <v>274</v>
+      </c>
+      <c r="C69" s="31"/>
+      <c r="D69" s="31" t="s">
+        <v>297</v>
       </c>
       <c r="E69" s="54">
         <f t="shared" si="13"/>
@@ -13574,11 +13531,9 @@
         <f t="shared" si="14"/>
         <v>R-SW*Att_GAS*</v>
       </c>
-      <c r="C70" s="30" t="s">
-        <v>298</v>
-      </c>
-      <c r="D70" s="30">
-        <v>1</v>
+      <c r="C70" s="30"/>
+      <c r="D70" s="30" t="s">
+        <v>297</v>
       </c>
       <c r="E70" s="53">
         <f t="shared" si="13"/>
@@ -13603,11 +13558,9 @@
         <f t="shared" si="14"/>
         <v>R-SW*Att_PEA*</v>
       </c>
-      <c r="C71" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="D71" s="31">
-        <v>1</v>
+      <c r="C71" s="31"/>
+      <c r="D71" s="31" t="s">
+        <v>297</v>
       </c>
       <c r="E71" s="54">
         <f t="shared" si="13"/>
@@ -13632,11 +13585,9 @@
         <f t="shared" si="14"/>
         <v>R-SW*Att_SMF*</v>
       </c>
-      <c r="C72" s="30" t="s">
-        <v>298</v>
-      </c>
-      <c r="D72" s="30">
-        <v>1</v>
+      <c r="C72" s="30"/>
+      <c r="D72" s="30" t="s">
+        <v>297</v>
       </c>
       <c r="E72" s="53">
         <f t="shared" si="13"/>
@@ -13661,11 +13612,9 @@
         <f t="shared" si="14"/>
         <v>R-SW*Att_WOO*</v>
       </c>
-      <c r="C73" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="D73" s="31">
-        <v>1</v>
+      <c r="C73" s="31"/>
+      <c r="D73" s="31" t="s">
+        <v>297</v>
       </c>
       <c r="E73" s="54">
         <f t="shared" si="13"/>
@@ -13687,13 +13636,11 @@
         <v>198</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="C74" s="30" t="s">
-        <v>298</v>
-      </c>
-      <c r="D74" s="30">
-        <v>1</v>
+        <v>270</v>
+      </c>
+      <c r="C74" s="30"/>
+      <c r="D74" s="30" t="s">
+        <v>297</v>
       </c>
       <c r="E74" s="53">
         <f t="shared" si="13"/>
@@ -13711,11 +13658,9 @@
         <f t="shared" si="14"/>
         <v>R-SW*Att_HET*</v>
       </c>
-      <c r="C75" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="D75" s="31">
-        <v>1</v>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31" t="s">
+        <v>297</v>
       </c>
       <c r="E75" s="54">
         <f t="shared" si="13"/>
@@ -13753,11 +13698,9 @@
         <f>"R-SW*"&amp;G77&amp;"_"&amp;H77&amp;"*"</f>
         <v>R-SW*Det_COA*</v>
       </c>
-      <c r="C77" s="30" t="s">
-        <v>300</v>
-      </c>
-      <c r="D77" s="30">
-        <v>1</v>
+      <c r="C77" s="30"/>
+      <c r="D77" s="30" t="s">
+        <v>298</v>
       </c>
       <c r="E77" s="53">
         <f>E34</f>
@@ -13782,11 +13725,9 @@
         <f>"R-SW*"&amp;G78&amp;"_"&amp;H78&amp;"*"</f>
         <v>R-SW*Det_BDL*</v>
       </c>
-      <c r="C78" s="31" t="s">
-        <v>300</v>
-      </c>
-      <c r="D78" s="31">
-        <v>1</v>
+      <c r="C78" s="31"/>
+      <c r="D78" s="31" t="s">
+        <v>298</v>
       </c>
       <c r="E78" s="54">
         <f t="shared" ref="E78:E90" si="17">E35</f>
@@ -13811,11 +13752,9 @@
         <f>"R-SW*"&amp;G79&amp;"_"&amp;H79&amp;"*"</f>
         <v>R-SW*Det_ETH*</v>
       </c>
-      <c r="C79" s="30" t="s">
-        <v>300</v>
-      </c>
-      <c r="D79" s="30">
-        <v>1</v>
+      <c r="C79" s="30"/>
+      <c r="D79" s="30" t="s">
+        <v>298</v>
       </c>
       <c r="E79" s="53">
         <f t="shared" si="17"/>
@@ -13840,11 +13779,9 @@
         <f>"R-SW*"&amp;G80&amp;"_"&amp;H80&amp;"*"</f>
         <v>R-SW*Det_LPG*</v>
       </c>
-      <c r="C80" s="31" t="s">
-        <v>300</v>
-      </c>
-      <c r="D80" s="31">
-        <v>1</v>
+      <c r="C80" s="31"/>
+      <c r="D80" s="31" t="s">
+        <v>298</v>
       </c>
       <c r="E80" s="54">
         <f t="shared" si="17"/>
@@ -13869,11 +13806,9 @@
         <f>"R-SW_"&amp;G81&amp;"*"&amp;"HPN*"</f>
         <v>R-SW_Det*HPN*</v>
       </c>
-      <c r="C81" s="30" t="s">
-        <v>300</v>
-      </c>
-      <c r="D81" s="30">
-        <v>1</v>
+      <c r="C81" s="30"/>
+      <c r="D81" s="30" t="s">
+        <v>298</v>
       </c>
       <c r="E81" s="53">
         <f t="shared" si="17"/>
@@ -13898,11 +13833,9 @@
         <f>"R-SW_"&amp;G82&amp;"_"&amp;H82&amp;"_N1"</f>
         <v>R-SW_Det_ELC_N1</v>
       </c>
-      <c r="C82" s="31" t="s">
-        <v>300</v>
-      </c>
-      <c r="D82" s="31">
-        <v>1</v>
+      <c r="C82" s="31"/>
+      <c r="D82" s="31" t="s">
+        <v>298</v>
       </c>
       <c r="E82" s="54">
         <f t="shared" si="17"/>
@@ -13927,11 +13860,9 @@
         <f t="shared" ref="B83:B90" si="18">"R-SW*"&amp;G83&amp;"_"&amp;H83&amp;"*"</f>
         <v>R-SW*Det_KER*</v>
       </c>
-      <c r="C83" s="30" t="s">
-        <v>300</v>
-      </c>
-      <c r="D83" s="30">
-        <v>1</v>
+      <c r="C83" s="30"/>
+      <c r="D83" s="30" t="s">
+        <v>298</v>
       </c>
       <c r="E83" s="53">
         <f t="shared" si="17"/>
@@ -13953,13 +13884,11 @@
         <v>198</v>
       </c>
       <c r="B84" s="31" t="s">
-        <v>276</v>
-      </c>
-      <c r="C84" s="31" t="s">
-        <v>300</v>
-      </c>
-      <c r="D84" s="31">
-        <v>1</v>
+        <v>275</v>
+      </c>
+      <c r="C84" s="31"/>
+      <c r="D84" s="31" t="s">
+        <v>298</v>
       </c>
       <c r="E84" s="54">
         <f t="shared" si="17"/>
@@ -13977,11 +13906,9 @@
         <f t="shared" si="18"/>
         <v>R-SW*Det_GAS*</v>
       </c>
-      <c r="C85" s="30" t="s">
-        <v>300</v>
-      </c>
-      <c r="D85" s="30">
-        <v>1</v>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30" t="s">
+        <v>298</v>
       </c>
       <c r="E85" s="53">
         <f t="shared" si="17"/>
@@ -14006,11 +13933,9 @@
         <f t="shared" si="18"/>
         <v>R-SW*Det_PEA*</v>
       </c>
-      <c r="C86" s="31" t="s">
-        <v>300</v>
-      </c>
-      <c r="D86" s="31">
-        <v>1</v>
+      <c r="C86" s="31"/>
+      <c r="D86" s="31" t="s">
+        <v>298</v>
       </c>
       <c r="E86" s="54">
         <f t="shared" si="17"/>
@@ -14035,11 +13960,9 @@
         <f t="shared" si="18"/>
         <v>R-SW*Det_SMF*</v>
       </c>
-      <c r="C87" s="30" t="s">
-        <v>300</v>
-      </c>
-      <c r="D87" s="30">
-        <v>1</v>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30" t="s">
+        <v>298</v>
       </c>
       <c r="E87" s="53">
         <f t="shared" si="17"/>
@@ -14064,11 +13987,9 @@
         <f t="shared" si="18"/>
         <v>R-SW*Det_WOO*</v>
       </c>
-      <c r="C88" s="31" t="s">
-        <v>300</v>
-      </c>
-      <c r="D88" s="31">
-        <v>1</v>
+      <c r="C88" s="31"/>
+      <c r="D88" s="31" t="s">
+        <v>298</v>
       </c>
       <c r="E88" s="54">
         <f t="shared" si="17"/>
@@ -14090,13 +14011,11 @@
         <v>198</v>
       </c>
       <c r="B89" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="C89" s="30" t="s">
-        <v>300</v>
-      </c>
-      <c r="D89" s="30">
-        <v>1</v>
+        <v>271</v>
+      </c>
+      <c r="C89" s="30"/>
+      <c r="D89" s="30" t="s">
+        <v>298</v>
       </c>
       <c r="E89" s="53">
         <f t="shared" si="17"/>
@@ -14114,11 +14033,9 @@
         <f t="shared" si="18"/>
         <v>R-SW*Det_HET*</v>
       </c>
-      <c r="C90" s="31" t="s">
-        <v>300</v>
-      </c>
-      <c r="D90" s="31">
-        <v>1</v>
+      <c r="C90" s="31"/>
+      <c r="D90" s="31" t="s">
+        <v>298</v>
       </c>
       <c r="E90" s="54">
         <f t="shared" si="17"/>
@@ -15182,11 +15099,10 @@
         <f>"R-HC_"&amp;G135&amp;"_"&amp;H135&amp;"_HPN*"</f>
         <v>R-HC_Apt_ELC_HPN*</v>
       </c>
-      <c r="C135" s="30" t="str">
-        <f>"RSDSC_"&amp;G135</f>
-        <v>RSDSC_Apt</v>
-      </c>
-      <c r="D135" s="30"/>
+      <c r="C135" s="30"/>
+      <c r="D135" s="30" t="s">
+        <v>299</v>
+      </c>
       <c r="E135" s="53">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,I135,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>0.18130269923092601</v>
@@ -15210,11 +15126,10 @@
         <f>"R-HC_"&amp;G136&amp;"_"&amp;H136&amp;"_HPN*"</f>
         <v>R-HC_Att_ELC_HPN*</v>
       </c>
-      <c r="C136" s="31" t="str">
-        <f>"RSDSC_"&amp;G136</f>
-        <v>RSDSC_Att</v>
-      </c>
-      <c r="D136" s="31"/>
+      <c r="C136" s="31"/>
+      <c r="D136" s="31" t="s">
+        <v>300</v>
+      </c>
       <c r="E136" s="54">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,I136,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>0.11404303534564</v>
@@ -15238,11 +15153,10 @@
         <f>"R-HC_"&amp;G137&amp;"_"&amp;H137&amp;"_HPN*"</f>
         <v>R-HC_Det_ELC_HPN*</v>
       </c>
-      <c r="C137" s="30" t="str">
-        <f>"RSDSC_"&amp;G137</f>
-        <v>RSDSC_Det</v>
-      </c>
-      <c r="D137" s="30"/>
+      <c r="C137" s="30"/>
+      <c r="D137" s="30" t="s">
+        <v>301</v>
+      </c>
       <c r="E137" s="53">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,I137,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>0.138319067250922</v>
@@ -15255,106 +15169,6 @@
       </c>
       <c r="I137" s="30" t="str">
         <f t="shared" si="30"/>
-        <v>R-SH_Det_ELC*X1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A138" s="27" t="s">
-        <v>252</v>
-      </c>
-      <c r="B138" s="28"/>
-      <c r="C138" s="29"/>
-      <c r="D138" s="29"/>
-      <c r="E138" s="56"/>
-      <c r="F138" s="28"/>
-      <c r="G138" s="28"/>
-      <c r="H138" s="28"/>
-      <c r="I138" s="28"/>
-    </row>
-    <row r="139" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A139" s="30" t="s">
-        <v>245</v>
-      </c>
-      <c r="B139" s="30" t="str">
-        <f>"R-HC_"&amp;G139&amp;"_"&amp;H139&amp;"_HPN*"</f>
-        <v>R-HC_Apt_ELC_HPN*</v>
-      </c>
-      <c r="C139" s="30" t="s">
-        <v>295</v>
-      </c>
-      <c r="D139" s="30">
-        <v>1</v>
-      </c>
-      <c r="E139" s="53">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,I139,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.18130269923092601</v>
-      </c>
-      <c r="G139" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="H139" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="I139" s="30" t="str">
-        <f t="shared" ref="I139:I141" si="31">"R-SH_"&amp;G139&amp;"_"&amp;H139&amp;"*X1"</f>
-        <v>R-SH_Apt_ELC*X1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A140" s="31" t="s">
-        <v>245</v>
-      </c>
-      <c r="B140" s="31" t="str">
-        <f>"R-HC_"&amp;G140&amp;"_"&amp;H140&amp;"_HPN*"</f>
-        <v>R-HC_Att_ELC_HPN*</v>
-      </c>
-      <c r="C140" s="31" t="s">
-        <v>297</v>
-      </c>
-      <c r="D140" s="31">
-        <v>1</v>
-      </c>
-      <c r="E140" s="54">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,I140,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.11404303534564</v>
-      </c>
-      <c r="G140" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="H140" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="I140" s="31" t="str">
-        <f t="shared" si="31"/>
-        <v>R-SH_Att_ELC*X1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A141" s="30" t="s">
-        <v>245</v>
-      </c>
-      <c r="B141" s="30" t="str">
-        <f>"R-HC_"&amp;G141&amp;"_"&amp;H141&amp;"_HPN*"</f>
-        <v>R-HC_Det_ELC_HPN*</v>
-      </c>
-      <c r="C141" s="30" t="s">
-        <v>299</v>
-      </c>
-      <c r="D141" s="30">
-        <v>1</v>
-      </c>
-      <c r="E141" s="53">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,I141,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.138319067250922</v>
-      </c>
-      <c r="G141" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="H141" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="I141" s="30" t="str">
-        <f t="shared" si="31"/>
         <v>R-SH_Det_ELC*X1</v>
       </c>
     </row>
@@ -15679,7 +15493,7 @@
         <v>R-S*_Apt_*HET*</v>
       </c>
       <c r="G16" s="30" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -15964,7 +15778,7 @@
         <v>R-S*_Att_*HET*</v>
       </c>
       <c r="G29" s="30" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -16249,7 +16063,7 @@
         <v>R-S*_Det_*HET*</v>
       </c>
       <c r="G42" s="30" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -16636,7 +16450,7 @@
         <v>R-WH_Apt_HET*</v>
       </c>
       <c r="G60" s="30" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -16944,7 +16758,7 @@
         <v>R-WH_Att_HET*</v>
       </c>
       <c r="G74" s="30" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -17252,7 +17066,7 @@
         <v>R-WH_Det_HET*</v>
       </c>
       <c r="G88" s="30" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -18864,7 +18678,7 @@
         <v>78</v>
       </c>
       <c r="C39" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D39" t="s">
         <v>131</v>
@@ -19701,7 +19515,7 @@
         <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D19" t="s">
         <v>131</v>
@@ -19742,7 +19556,7 @@
         <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D20" t="s">
         <v>131</v>
@@ -19783,7 +19597,7 @@
         <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D21" t="s">
         <v>131</v>
@@ -19865,7 +19679,7 @@
         <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D23" t="s">
         <v>131</v>
@@ -19906,7 +19720,7 @@
         <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D24" t="s">
         <v>131</v>
@@ -19947,7 +19761,7 @@
         <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D25" t="s">
         <v>131</v>
@@ -20193,7 +20007,7 @@
         <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D31" t="s">
         <v>131</v>
@@ -20234,7 +20048,7 @@
         <v>78</v>
       </c>
       <c r="C32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D32" t="s">
         <v>131</v>
@@ -20275,7 +20089,7 @@
         <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D33" t="s">
         <v>131</v>
@@ -20357,7 +20171,7 @@
         <v>78</v>
       </c>
       <c r="C35" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D35" t="s">
         <v>131</v>
@@ -20398,7 +20212,7 @@
         <v>78</v>
       </c>
       <c r="C36" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D36" t="s">
         <v>131</v>
@@ -20439,7 +20253,7 @@
         <v>78</v>
       </c>
       <c r="C37" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D37" t="s">
         <v>131</v>

</xml_diff>